<commit_message>
-show/hide '--' event type
-remove event type defaults button
-help update (issue #486)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/programs.xlsx
+++ b/doc/help_dialogs/Input_files/programs.xlsx
@@ -14,35 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>EXTERNAL PROGRAMS</t>
   </si>
   <si>
-    <t>tn:Allows to link to external programs that print temperature when called</t>
-  </si>
-  <si>
     <t>tn:</t>
   </si>
   <si>
-    <t>tn:The output of the program must be to Stdout (like when using print statements)</t>
-  </si>
-  <si>
-    <t>tn:this allo ws to connect meters that use any programming language</t>
-  </si>
-  <si>
-    <t>tn:Example of output needed from program for single temperature (BT)</t>
-  </si>
-  <si>
-    <t>tn:"100.4" (note: "" not needed)</t>
-  </si>
-  <si>
-    <t>tn:Example of output needed from program for double temperature (ET,BT)</t>
-  </si>
-  <si>
-    <t>tn:"200.4,100.4" (note: temperatures are separated by a comma "ET,BT")</t>
-  </si>
-  <si>
     <t>bn:Example of a file written in python language called test.py:</t>
   </si>
   <si>
@@ -56,14 +35,61 @@
   </si>
   <si>
     <t>bn:print ("237.1,100.4")</t>
+  </si>
+  <si>
+    <t>tn:Example of output needed from program for single temperature (BT):
+"100.4" (note: "" not needed)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tn:Link external programs that print temperature when called.  This allows to connect meters that use any program language.
+Artisan will start the program each sample period.  The program output must </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be to Stdout (like when using print statements).  The program must exit and must not be persistent.</t>
+    </r>
+  </si>
+  <si>
+    <t>tn:Data may also be provided to the "Program" extra devices.  Extra device "Program" are the first two values, typically ET and BT.  "Program 34" are the third and fourth values.  Up to 10 values may be supplied.</t>
+  </si>
+  <si>
+    <t>tn:If only one termperature is provided it will be interpreted as BT.  If more than one temperature is provided the values are order dependent with ET first and BT second.</t>
+  </si>
+  <si>
+    <t>tn:Example of output needed from program for double temperature (ET,BT)
+"200.4,100.4" (note: temperatures are separated by a comma "ET,BT")</t>
+  </si>
+  <si>
+    <t>tn:Example of output needed from program for double temperature (ET,BT) and extra devices (Program and Program 34)
+"200.4,100.4,312.4,345.6,299.0,275.5"</t>
+  </si>
+  <si>
+    <t>bn:Note: In many cases the path to the Python or other language executatable should be provided along with the external program path.  On Windows it is  advised to enclose the paths with quotation marks if there are any spaces, and use forward slashes '/' in the path.
+"C:/Python38-64/python.exe" "c:/scripts/test.py"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,8 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,106 +423,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="100.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
+      <c r="A5" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
+      <c r="A7" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
+      <c r="A15" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>